<commit_message>
Add and comment out library(maftools)
</commit_message>
<xml_diff>
--- a/analyses/tumor-clone-inference/results/signif_genes_edited.xlsx
+++ b/analyses/tumor-clone-inference/results/signif_genes_edited.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chronia/CHOP/GitHub/pbta-tumor-evolution/analyses/tumor-clone-inference/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B30CF06-D546-7A46-9AEF-0E06C4E106FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FCD56F-3C2D-F04C-A1E9-5A49273976B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11940" yWindow="3880" windowWidth="29180" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signif_genes" sheetId="1" r:id="rId1"/>
@@ -1247,7 +1247,7 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>